<commit_message>
Hinzufügen von eig. Histogramm(Achsen)
</commit_message>
<xml_diff>
--- a/doku/sonstige/GANTT-Diagramm.xlsx
+++ b/doku/sonstige/GANTT-Diagramm.xlsx
@@ -314,11 +314,11 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="4" fillId="8" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="8" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -409,24 +409,24 @@
   </sheetPr>
   <dimension ref="A1:Y20"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="X11" activeCellId="0" sqref="X11"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="V12" activeCellId="0" sqref="V12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="28.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="2" style="0" width="4.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="5.34"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="4.55"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="5.35"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="4.56"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="4.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="0" width="4"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="0" width="3.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="0" width="4.22"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="0" width="4.55"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="0" width="4.56"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="24" style="0" width="4.89"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="25" style="0" width="4.44"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="26" style="0" width="3.89"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="29" min="27" style="0" width="4.55"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="29" min="27" style="0" width="4.56"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="30" style="0" width="10.55"/>
   </cols>
   <sheetData>
@@ -636,8 +636,8 @@
       <c r="H6" s="8"/>
       <c r="I6" s="8"/>
       <c r="J6" s="8"/>
-      <c r="K6" s="9"/>
-      <c r="L6" s="7"/>
+      <c r="K6" s="11"/>
+      <c r="L6" s="11"/>
       <c r="M6" s="7"/>
       <c r="N6" s="10"/>
       <c r="O6" s="10"/>
@@ -667,7 +667,7 @@
       <c r="J7" s="8"/>
       <c r="K7" s="9"/>
       <c r="L7" s="11"/>
-      <c r="M7" s="7"/>
+      <c r="M7" s="11"/>
       <c r="N7" s="10"/>
       <c r="O7" s="10"/>
       <c r="P7" s="12"/>
@@ -812,11 +812,11 @@
       <c r="H12" s="8"/>
       <c r="I12" s="8"/>
       <c r="J12" s="8"/>
-      <c r="K12" s="9"/>
+      <c r="K12" s="17"/>
       <c r="L12" s="13"/>
       <c r="M12" s="13"/>
       <c r="N12" s="7"/>
-      <c r="O12" s="17"/>
+      <c r="O12" s="18"/>
       <c r="P12" s="10"/>
       <c r="Q12" s="10"/>
       <c r="R12" s="10"/>
@@ -846,7 +846,7 @@
       <c r="M13" s="13"/>
       <c r="N13" s="7"/>
       <c r="O13" s="10"/>
-      <c r="P13" s="18"/>
+      <c r="P13" s="17"/>
       <c r="Q13" s="10"/>
       <c r="R13" s="10"/>
       <c r="S13" s="19"/>
@@ -875,8 +875,8 @@
       <c r="M14" s="13"/>
       <c r="N14" s="7"/>
       <c r="O14" s="10"/>
-      <c r="P14" s="18"/>
-      <c r="Q14" s="18"/>
+      <c r="P14" s="17"/>
+      <c r="Q14" s="17"/>
       <c r="R14" s="10"/>
       <c r="S14" s="19"/>
       <c r="T14" s="10"/>
@@ -905,8 +905,8 @@
       <c r="N15" s="7"/>
       <c r="O15" s="10"/>
       <c r="P15" s="10"/>
-      <c r="Q15" s="18"/>
-      <c r="R15" s="18"/>
+      <c r="Q15" s="17"/>
+      <c r="R15" s="17"/>
       <c r="S15" s="19"/>
       <c r="T15" s="10"/>
       <c r="U15" s="10"/>
@@ -935,8 +935,8 @@
       <c r="O16" s="10"/>
       <c r="P16" s="10"/>
       <c r="Q16" s="10"/>
-      <c r="R16" s="18"/>
-      <c r="S16" s="18"/>
+      <c r="R16" s="17"/>
+      <c r="S16" s="17"/>
       <c r="T16" s="10"/>
       <c r="U16" s="10"/>
       <c r="V16" s="10"/>

</xml_diff>